<commit_message>
Added Chat_ID parameter to All casters
-Added the ChatDataBaseID property to the CasterStats class, causing all ICasters to have a chat ID.
-In most cases, this chatID is readonly, but the property is overridden to be read/write in PlayerStats (so the player's lines can change over the course of the game
-Added fields to databases and parses to add chat_id fields to the ally and enemy databases
-Removed all double quotes from chat lines (to remove excel formatting)

FILES MODIFIED

CasterStats.cs, BattleManager.cs, Player.cs, Enemy.cs, Ally.cs, EnemyDatabase.cs/xlsl/txt, AllyDatabase.cs/xlsl/txt, ChatDatabase.cs/xlsl/txt,
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/allyDatabase.xlsx
+++ b/Typocrypha/Assets/excel/allyDatabase.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>ATK</t>
   </si>
@@ -60,19 +60,22 @@
     <t>Dahlia</t>
   </si>
   <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Uber_Illyia</t>
+  </si>
+  <si>
+    <t>max_hp (inertia)</t>
+  </si>
+  <si>
+    <t>max_shield</t>
+  </si>
+  <si>
     <t>ID</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Uber_Illyia</t>
-  </si>
-  <si>
-    <t>max_hp (inertia)</t>
-  </si>
-  <si>
-    <t>max_shield</t>
+    <t>chat_id</t>
   </si>
 </sst>
 </file>
@@ -913,190 +916,200 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.5546875" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
-    <col min="11" max="11" width="9.6640625" customWidth="1"/>
-    <col min="12" max="12" width="9.88671875" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" customWidth="1"/>
-    <col min="14" max="14" width="13.33203125" customWidth="1"/>
+    <col min="1" max="2" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="12" max="12" width="9.6640625" customWidth="1"/>
+    <col min="13" max="13" width="9.88671875" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" t="s">
-        <v>1</v>
-      </c>
       <c r="H1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>3</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>4</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>5</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>6</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2">
         <v>100</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>10</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>2</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
       <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
         <v>0.1</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
         <v>10</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>0</v>
       </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
       <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
         <v>1.5</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3">
         <v>100</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>10</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>3</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
       <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
         <v>0.1</v>
       </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
         <v>5</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>1.2</v>
       </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
       <c r="M3">
         <v>1</v>
       </c>
       <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
         <v>200</v>
-      </c>
-      <c r="D4">
-        <v>10</v>
       </c>
       <c r="E4">
         <v>10</v>
       </c>
       <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="G4">
         <v>50</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0.9</v>
       </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
         <v>30</v>
       </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
       <c r="L4">
         <v>1</v>
       </c>
@@ -1106,8 +1119,11 @@
       <c r="N4">
         <v>1</v>
       </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>

</xml_diff>